<commit_message>
update logic import store new
</commit_message>
<xml_diff>
--- a/mydata/import-store.xlsx
+++ b/mydata/import-store.xlsx
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D49" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +655,7 @@
         <v>11</v>
       </c>
       <c r="I9" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -995,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="4:10" x14ac:dyDescent="0.3">
@@ -1015,7 +1015,7 @@
         <v>11</v>
       </c>
       <c r="I27" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="4:10" x14ac:dyDescent="0.3">
@@ -1035,7 +1035,7 @@
         <v>11</v>
       </c>
       <c r="I28" s="3">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.3">
@@ -1212,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
@@ -1332,7 +1332,7 @@
         <v>11</v>
       </c>
       <c r="I45" s="3">
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
@@ -1412,7 +1412,7 @@
         <v>11</v>
       </c>
       <c r="I49" s="3">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="4:10" x14ac:dyDescent="0.3">

</xml_diff>